<commit_message>
Fix build and push updated site
</commit_message>
<xml_diff>
--- a/estimates_PS2025.xlsx
+++ b/estimates_PS2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\tibor-pal.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25A7751B-2700-4E8F-997C-138AA5DC90D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75143D5B-72C5-4B8F-8770-7396E9090229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{898E4DB8-E74C-49BD-9493-76D0D230C2FB}"/>
   </bookViews>
@@ -458,7 +458,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +527,7 @@
         <v>4.0038986779857198E-2</v>
       </c>
       <c r="I2">
-        <v>0.52213625254846396</v>
+        <v>0.65962561574593104</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -556,7 +556,7 @@
         <v>3.98916450777132E-2</v>
       </c>
       <c r="I3">
-        <v>0.48029331887383597</v>
+        <v>0.64181220342381595</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -585,7 +585,7 @@
         <v>3.97146429777262E-2</v>
       </c>
       <c r="I4">
-        <v>0.46375864238998499</v>
+        <v>0.60811598362900099</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -614,7 +614,7 @@
         <v>3.9813716405990601E-2</v>
       </c>
       <c r="I5">
-        <v>0.43759595294819797</v>
+        <v>0.58284537588402097</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -643,7 +643,7 @@
         <v>3.9762288557270702E-2</v>
       </c>
       <c r="I6">
-        <v>0.41441290446373402</v>
+        <v>0.59935617961070997</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -672,7 +672,7 @@
         <v>3.9760494105272701E-2</v>
       </c>
       <c r="I7">
-        <v>0.37229504954506798</v>
+        <v>0.57945958317593105</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -701,7 +701,7 @@
         <v>3.9730993844109198E-2</v>
       </c>
       <c r="I8">
-        <v>0.34219873218938601</v>
+        <v>0.55893492422101199</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -730,7 +730,7 @@
         <v>3.9626157456553901E-2</v>
       </c>
       <c r="I9">
-        <v>0.36171783003754499</v>
+        <v>0.53852644184068199</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -759,7 +759,7 @@
         <v>3.9656903718199903E-2</v>
       </c>
       <c r="I10">
-        <v>0.33826340853442399</v>
+        <v>0.545670806575279</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -788,7 +788,7 @@
         <v>3.96840639471936E-2</v>
       </c>
       <c r="I11">
-        <v>0.31489824951394801</v>
+        <v>0.52768104802566196</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -817,7 +817,7 @@
         <v>3.9697075264022399E-2</v>
       </c>
       <c r="I12">
-        <v>0.29250072856158599</v>
+        <v>0.55557395268487797</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -846,7 +846,7 @@
         <v>3.9880689680378799E-2</v>
       </c>
       <c r="I13">
-        <v>0.30024662914851602</v>
+        <v>0.55177203374608896</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -875,7 +875,7 @@
         <v>3.9804988468630897E-2</v>
       </c>
       <c r="I14">
-        <v>0.28093728844546101</v>
+        <v>0.54948954769159297</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -904,7 +904,7 @@
         <v>3.9475776211299503E-2</v>
       </c>
       <c r="I15">
-        <v>0.31115241690189899</v>
+        <v>0.53705184337911904</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -933,7 +933,7 @@
         <v>3.92773391320742E-2</v>
       </c>
       <c r="I16">
-        <v>0.30694237722429502</v>
+        <v>0.52459043069866895</v>
       </c>
       <c r="L16" s="1"/>
     </row>
@@ -963,7 +963,7 @@
         <v>3.9044937638487702E-2</v>
       </c>
       <c r="I17">
-        <v>0.30442876302231098</v>
+        <v>0.50968945011984801</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -992,7 +992,7 @@
         <v>3.91572243973883E-2</v>
       </c>
       <c r="I18">
-        <v>0.29091468247690999</v>
+        <v>0.49476933874187101</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1021,7 +1021,7 @@
         <v>3.90079117217315E-2</v>
       </c>
       <c r="I19">
-        <v>0.27768511998061501</v>
+        <v>0.515393296041745</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1050,7 +1050,7 @@
         <v>3.8906912559505999E-2</v>
       </c>
       <c r="I20">
-        <v>0.26227333556347299</v>
+        <v>0.78172482979352897</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1079,7 +1079,7 @@
         <v>3.8855155381478601E-2</v>
       </c>
       <c r="I21">
-        <v>0.24728669855906801</v>
+        <v>0.74096631821958103</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
         <v>3.9233360120331601E-2</v>
       </c>
       <c r="I22">
-        <v>0.26812024960477399</v>
+        <v>0.70135676722738904</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
         <v>4.0449754319989303E-2</v>
       </c>
       <c r="I23">
-        <v>0.61358370951572205</v>
+        <v>0.82243878167267004</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1166,7 +1166,7 @@
         <v>4.0637075046256903E-2</v>
       </c>
       <c r="I24">
-        <v>0.55152108473588202</v>
+        <v>0.76043746079213403</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1195,7 +1195,7 @@
         <v>4.0792947968521599E-2</v>
       </c>
       <c r="I25">
-        <v>0.49439131493565402</v>
+        <v>0.73937967210951105</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1224,7 +1224,7 @@
         <v>4.0223488867603997E-2</v>
       </c>
       <c r="I26">
-        <v>0.67889554959922604</v>
+        <v>0.71521055306372106</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1253,7 +1253,7 @@
         <v>4.0165154962069897E-2</v>
       </c>
       <c r="I27">
-        <v>0.58075513177598803</v>
+        <v>0.72585117873397798</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1282,7 +1282,7 @@
         <v>4.0365423878773302E-2</v>
       </c>
       <c r="I28">
-        <v>0.549172299528768</v>
+        <v>0.68579506985204597</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1311,7 +1311,7 @@
         <v>4.05532872386506E-2</v>
       </c>
       <c r="I29">
-        <v>0.51401613521371403</v>
+        <v>0.64915628366619604</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1340,7 +1340,7 @@
         <v>4.0822271095020103E-2</v>
       </c>
       <c r="I30">
-        <v>0.529349933669505</v>
+        <v>0.61357193047514902</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1369,7 +1369,7 @@
         <v>4.0930565618132297E-2</v>
       </c>
       <c r="I31">
-        <v>0.47280487783337299</v>
+        <v>0.60886599373302996</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1398,7 +1398,7 @@
         <v>4.0825743113149897E-2</v>
       </c>
       <c r="I32">
-        <v>0.42389388062330602</v>
+        <v>0.58003057881120901</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1427,7 +1427,7 @@
         <v>4.0809763741119602E-2</v>
       </c>
       <c r="I33">
-        <v>0.37896051386700103</v>
+        <v>0.56572071921405498</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1456,7 +1456,7 @@
         <v>4.0565091853868099E-2</v>
       </c>
       <c r="I34">
-        <v>0.37320779832451001</v>
+        <v>0.54413417569469702</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1485,7 +1485,7 @@
         <v>4.0601152931549901E-2</v>
       </c>
       <c r="I35">
-        <v>0.33892547235606602</v>
+        <v>0.55476929117707696</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1514,7 +1514,7 @@
         <v>4.0437299972004598E-2</v>
       </c>
       <c r="I36">
-        <v>0.32252993214806802</v>
+        <v>0.53446377168519599</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1543,7 +1543,7 @@
         <v>4.0372649181884102E-2</v>
       </c>
       <c r="I37">
-        <v>0.298572001158948</v>
+        <v>0.52127133569453299</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1572,7 +1572,7 @@
         <v>4.0144178753061997E-2</v>
       </c>
       <c r="I38">
-        <v>0.31025896643311701</v>
+        <v>0.66180292811227204</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1601,7 +1601,7 @@
         <v>4.01020571092216E-2</v>
       </c>
       <c r="I39">
-        <v>0.28814152324396602</v>
+        <v>0.62792247889644903</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1630,7 +1630,7 @@
         <v>4.0037837295723501E-2</v>
       </c>
       <c r="I40">
-        <v>0.27421380541676299</v>
+        <v>0.62543453577484398</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1659,7 +1659,7 @@
         <v>4.0371756936773598E-2</v>
       </c>
       <c r="I41">
-        <v>0.44047311565797698</v>
+        <v>0.72746054169371099</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1688,7 +1688,7 @@
         <v>4.0338404993010502E-2</v>
       </c>
       <c r="I42">
-        <v>0.39677663950346198</v>
+        <v>1.17372946673889</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1717,7 +1717,7 @@
         <v>4.0226195933245001E-2</v>
       </c>
       <c r="I43">
-        <v>0.393658358539895</v>
+        <v>1.06498862028566</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -1746,7 +1746,7 @@
         <v>4.0038437852588399E-2</v>
       </c>
       <c r="I44">
-        <v>0.53168883972130798</v>
+        <v>1.02298998644423</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -1775,7 +1775,7 @@
         <v>3.9834848184443702E-2</v>
       </c>
       <c r="I45">
-        <v>1.38013086109115</v>
+        <v>0.920948299118027</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -1804,7 +1804,7 @@
         <v>3.98502639132561E-2</v>
       </c>
       <c r="I46">
-        <v>1.13669076133796</v>
+        <v>0.85884053148266004</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -1833,7 +1833,7 @@
         <v>3.9812554309181E-2</v>
       </c>
       <c r="I47">
-        <v>1.0489985123651699</v>
+        <v>0.78811421843860296</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -1862,7 +1862,7 @@
         <v>3.9811324489725498E-2</v>
       </c>
       <c r="I48">
-        <v>0.85063576964838705</v>
+        <v>1.4825442426672999</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -1891,7 +1891,7 @@
         <v>3.9763867653441198E-2</v>
       </c>
       <c r="I49">
-        <v>0.74009705851741803</v>
+        <v>1.30221786827154</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -1920,7 +1920,7 @@
         <v>3.9754354541398397E-2</v>
       </c>
       <c r="I50">
-        <v>0.62361402130509103</v>
+        <v>1.1720098548912099</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -1949,7 +1949,7 @@
         <v>4.0197683357015998E-2</v>
       </c>
       <c r="I51">
-        <v>2.20042743146597</v>
+        <v>1.1703706903245701</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -1978,7 +1978,7 @@
         <v>4.0248653801225498E-2</v>
       </c>
       <c r="I52">
-        <v>1.69826137644568</v>
+        <v>1.8942614774772699</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2007,7 +2007,7 @@
         <v>4.0311556606257501E-2</v>
       </c>
       <c r="I53">
-        <v>1.37609709996212</v>
+        <v>1.8675319279010001</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2036,7 +2036,7 @@
         <v>4.0452344770014602E-2</v>
       </c>
       <c r="I54">
-        <v>1.3722575527708201</v>
+        <v>1.57795522814077</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2065,7 +2065,7 @@
         <v>4.06898274772945E-2</v>
       </c>
       <c r="I55">
-        <v>3.5907165450543799</v>
+        <v>1.49660483096528</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2094,7 +2094,7 @@
         <v>4.07645670040723E-2</v>
       </c>
       <c r="I56">
-        <v>3.4901655017296398</v>
+        <v>1.60956769687207</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2123,7 +2123,7 @@
         <v>4.0766042353253602E-2</v>
       </c>
       <c r="I57">
-        <v>2.4924327020167998</v>
+        <v>1.4607676032333901</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2152,7 +2152,7 @@
         <v>4.0731646084122101E-2</v>
       </c>
       <c r="I58">
-        <v>2.2423160200686101</v>
+        <v>1.2676457731487101</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2181,7 +2181,7 @@
         <v>4.0732289035939999E-2</v>
       </c>
       <c r="I59">
-        <v>2.5931981708140701</v>
+        <v>1.12849869670934</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2210,7 +2210,7 @@
         <v>4.0746494142740702E-2</v>
       </c>
       <c r="I60">
-        <v>2.1363319906562301</v>
+        <v>1.1183599643997399</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2239,7 +2239,7 @@
         <v>4.0749255562879901E-2</v>
       </c>
       <c r="I61">
-        <v>1.60941580618179</v>
+        <v>1.0325109585380801</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2268,7 +2268,7 @@
         <v>4.0742364248292397E-2</v>
       </c>
       <c r="I62">
-        <v>1.2759993084746799</v>
+        <v>0.92922828035531702</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2297,7 +2297,7 @@
         <v>4.0656817191781998E-2</v>
       </c>
       <c r="I63">
-        <v>1.25321900997219</v>
+        <v>0.86405377600750399</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2326,7 +2326,7 @@
         <v>4.0720663081081597E-2</v>
       </c>
       <c r="I64">
-        <v>1.06856887950123</v>
+        <v>0.80206578492811498</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -2355,7 +2355,7 @@
         <v>4.0730018275446797E-2</v>
       </c>
       <c r="I65">
-        <v>0.865955197012099</v>
+        <v>0.74603592073973202</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -2384,7 +2384,7 @@
         <v>4.0802497849030298E-2</v>
       </c>
       <c r="I66">
-        <v>0.74907892783282504</v>
+        <v>0.76817325425696803</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -2413,7 +2413,7 @@
         <v>4.0736488826463503E-2</v>
       </c>
       <c r="I67">
-        <v>0.64579952335235302</v>
+        <v>0.71319421641762404</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -2442,7 +2442,7 @@
         <v>4.07880942582073E-2</v>
       </c>
       <c r="I68">
-        <v>0.55905959503397995</v>
+        <v>0.68888191383659103</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -2471,7 +2471,7 @@
         <v>4.0474824082545199E-2</v>
       </c>
       <c r="I69">
-        <v>0.59258014855574104</v>
+        <v>0.64714070823810699</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -2500,7 +2500,7 @@
         <v>4.0460166802506303E-2</v>
       </c>
       <c r="I70">
-        <v>0.511135990331548</v>
+        <v>0.62097049558736395</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -2529,7 +2529,7 @@
         <v>4.06105722107995E-2</v>
       </c>
       <c r="I71">
-        <v>0.47704829121116399</v>
+        <v>1.01867453406626</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -2558,7 +2558,7 @@
         <v>4.0590405895867203E-2</v>
       </c>
       <c r="I72">
-        <v>0.42128109625891902</v>
+        <v>1.38819287198256</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -2587,7 +2587,7 @@
         <v>4.0744309312910301E-2</v>
       </c>
       <c r="I73">
-        <v>0.38809435639001599</v>
+        <v>1.2360692551152599</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -2616,7 +2616,7 @@
         <v>3.9849213394284697E-2</v>
       </c>
       <c r="I74">
-        <v>1.04018780635511</v>
+        <v>1.1308518324271499</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -2645,7 +2645,7 @@
         <v>4.0263832319168497E-2</v>
       </c>
       <c r="I75">
-        <v>1.9295694498231899</v>
+        <v>1.1675104745354501</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -2674,7 +2674,7 @@
         <v>4.0196591764588098E-2</v>
       </c>
       <c r="I76">
-        <v>1.5303572034411901</v>
+        <v>1.0460493889469</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -2703,7 +2703,7 @@
         <v>4.0291883598760202E-2</v>
       </c>
       <c r="I77">
-        <v>1.28131586690383</v>
+        <v>0.939745385308564</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -2732,7 +2732,7 @@
         <v>4.0485062360466499E-2</v>
       </c>
       <c r="I78">
-        <v>1.3655707081499899</v>
+        <v>0.89028397251334102</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -2761,7 +2761,7 @@
         <v>4.0428557531471801E-2</v>
       </c>
       <c r="I79">
-        <v>1.0967093241161701</v>
+        <v>0.85787332532124505</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -2790,7 +2790,7 @@
         <v>4.0422056193245397E-2</v>
       </c>
       <c r="I80">
-        <v>0.88561138920874205</v>
+        <v>0.968893267788839</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -2819,7 +2819,7 @@
         <v>4.04942460590276E-2</v>
       </c>
       <c r="I81">
-        <v>0.79509555171413404</v>
+        <v>0.92517972207629096</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -2848,7 +2848,7 @@
         <v>4.04033571084704E-2</v>
       </c>
       <c r="I82">
-        <v>0.73843664229773098</v>
+        <v>0.87521300579561601</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -2877,7 +2877,7 @@
         <v>4.02570449993171E-2</v>
       </c>
       <c r="I83">
-        <v>0.94124416436653502</v>
+        <v>0.97498284230941401</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -2906,7 +2906,7 @@
         <v>4.02460397617131E-2</v>
       </c>
       <c r="I84">
-        <v>0.85844751814116205</v>
+        <v>0.92784159604154504</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -2935,7 +2935,7 @@
         <v>4.0263558698614199E-2</v>
       </c>
       <c r="I85">
-        <v>0.76848780551379603</v>
+        <v>0.87641014937912098</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -2964,7 +2964,7 @@
         <v>4.0416457493298898E-2</v>
       </c>
       <c r="I86">
-        <v>0.95308154279774404</v>
+        <v>0.81620039546940104</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -2993,7 +2993,7 @@
         <v>4.0559750841283999E-2</v>
       </c>
       <c r="I87">
-        <v>0.86338002734492103</v>
+        <v>0.75437122934935896</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -3022,7 +3022,7 @@
         <v>4.0397531993454597E-2</v>
       </c>
       <c r="I88">
-        <v>0.77058474993473303</v>
+        <v>1.1547661284176201</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -3051,7 +3051,7 @@
         <v>4.0530050756970797E-2</v>
       </c>
       <c r="I89">
-        <v>0.66867308556440597</v>
+        <v>1.35778511156911</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -3080,7 +3080,7 @@
         <v>4.0587531840206102E-2</v>
       </c>
       <c r="I90">
-        <v>0.57156595167006197</v>
+        <v>1.3769511456905299</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -3109,7 +3109,7 @@
         <v>4.1639993751988999E-2</v>
       </c>
       <c r="I91">
-        <v>1.33597481134061</v>
+        <v>1.2120408101081499</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -3138,7 +3138,7 @@
         <v>4.1129396462225097E-2</v>
       </c>
       <c r="I92">
-        <v>1.8460704091987501</v>
+        <v>1.1112926811969299</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -3167,7 +3167,7 @@
         <v>4.1396299225506798E-2</v>
       </c>
       <c r="I93">
-        <v>1.8984844576184701</v>
+        <v>1.01366652048128</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -3196,7 +3196,7 @@
         <v>4.1338526296741201E-2</v>
       </c>
       <c r="I94">
-        <v>1.4715329253676099</v>
+        <v>0.94955340700621704</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -3225,7 +3225,7 @@
         <v>4.1215129826901703E-2</v>
       </c>
       <c r="I95">
-        <v>1.2374614232818499</v>
+        <v>1.29721817651959</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -3254,7 +3254,7 @@
         <v>4.1308847692834903E-2</v>
       </c>
       <c r="I96">
-        <v>1.0300098147446199</v>
+        <v>1.1984652832793801</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -3283,7 +3283,7 @@
         <v>4.1443286748202801E-2</v>
       </c>
       <c r="I97">
-        <v>0.90414167275711499</v>
+        <v>1.0819161557249799</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -3312,7 +3312,7 @@
         <v>4.0963939701170203E-2</v>
       </c>
       <c r="I98">
-        <v>1.6852649974928</v>
+        <v>1.0205731118596499</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -3341,7 +3341,7 @@
         <v>4.1079696243823099E-2</v>
       </c>
       <c r="I99">
-        <v>1.43880903522591</v>
+        <v>0.99340474687827596</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -3370,7 +3370,7 @@
         <v>4.0998657634003899E-2</v>
       </c>
       <c r="I100">
-        <v>1.1730325680187099</v>
+        <v>0.97322898564301397</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -3399,7 +3399,7 @@
         <v>4.11364631671342E-2</v>
       </c>
       <c r="I101">
-        <v>1.0440594766508899</v>
+        <v>0.88328921548640604</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -3428,7 +3428,7 @@
         <v>4.0960421509822299E-2</v>
       </c>
       <c r="I102">
-        <v>0.989342991120292</v>
+        <v>0.82566327281072305</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -3457,7 +3457,7 @@
         <v>4.11280920908575E-2</v>
       </c>
       <c r="I103">
-        <v>0.94966465849572901</v>
+        <v>0.78370008815479597</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -3486,7 +3486,7 @@
         <v>4.11643932858533E-2</v>
       </c>
       <c r="I104">
-        <v>0.78268983819459104</v>
+        <v>0.89892026862645902</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -3515,7 +3515,7 @@
         <v>4.1063805062390997E-2</v>
       </c>
       <c r="I105">
-        <v>0.68420984006851404</v>
+        <v>0.82449593664937404</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -3544,7 +3544,7 @@
         <v>4.1186513283411198E-2</v>
       </c>
       <c r="I106">
-        <v>0.61667582817383504</v>
+        <v>0.81109544431355796</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -3573,7 +3573,7 @@
         <v>4.0843552612969902E-2</v>
       </c>
       <c r="I107">
-        <v>0.81054764934746604</v>
+        <v>0.75157418917039898</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -3602,7 +3602,7 @@
         <v>4.0804283870319299E-2</v>
       </c>
       <c r="I108">
-        <v>0.68228354955132797</v>
+        <v>0.81149952238936995</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -3631,7 +3631,7 @@
         <v>4.06453845852245E-2</v>
       </c>
       <c r="I109">
-        <v>0.66036581978620901</v>
+        <v>0.75292213981738798</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -3660,7 +3660,7 @@
         <v>4.0611563086197101E-2</v>
       </c>
       <c r="I110">
-        <v>0.56735376182714303</v>
+        <v>0.70152860022192398</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -3689,7 +3689,7 @@
         <v>4.0406645839472899E-2</v>
       </c>
       <c r="I111">
-        <v>0.66102147483817597</v>
+        <v>0.65737320240356201</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -3718,7 +3718,7 @@
         <v>4.0376253722258303E-2</v>
       </c>
       <c r="I112">
-        <v>0.56938174862719404</v>
+        <v>0.67778573986906498</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -3747,7 +3747,7 @@
         <v>4.0355940147678501E-2</v>
       </c>
       <c r="I113">
-        <v>0.49463237692933198</v>
+        <v>0.71926133626573696</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -3776,7 +3776,7 @@
         <v>4.0354413514568303E-2</v>
       </c>
       <c r="I114">
-        <v>0.43462952723831499</v>
+        <v>0.68367442827548597</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -3805,7 +3805,7 @@
         <v>4.0479506875384597E-2</v>
       </c>
       <c r="I115">
-        <v>0.46188350916985599</v>
+        <v>0.75752350096658005</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -3834,7 +3834,7 @@
         <v>4.0645441557925099E-2</v>
       </c>
       <c r="I116">
-        <v>0.51982686984677395</v>
+        <v>0.71938115874402897</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -3863,7 +3863,7 @@
         <v>4.0578665658630997E-2</v>
       </c>
       <c r="I117">
-        <v>0.46990072387781201</v>
+        <v>0.67243530970402998</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -3892,7 +3892,7 @@
         <v>4.0338233655084398E-2</v>
       </c>
       <c r="I118">
-        <v>0.57633185451666402</v>
+        <v>0.67005569972605905</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -3921,7 +3921,7 @@
         <v>4.0265335786575797E-2</v>
       </c>
       <c r="I119">
-        <v>0.51999925155590099</v>
+        <v>0.63107542703628605</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -3950,7 +3950,7 @@
         <v>4.02736823726128E-2</v>
       </c>
       <c r="I120">
-        <v>0.45465924573675498</v>
+        <v>0.61611254147699201</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -3979,7 +3979,7 @@
         <v>4.0420238658137098E-2</v>
       </c>
       <c r="I121">
-        <v>0.45146464073537901</v>
+        <v>0.61156392881979704</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -4008,7 +4008,7 @@
         <v>4.0433079819836397E-2</v>
       </c>
       <c r="I122">
-        <v>0.40074619460902999</v>
+        <v>0.58304140587395104</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -4037,7 +4037,7 @@
         <v>4.0611964827663397E-2</v>
       </c>
       <c r="I123">
-        <v>0.38208466376523798</v>
+        <v>0.55737069916372695</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -4066,7 +4066,7 @@
         <v>4.0381449236786097E-2</v>
       </c>
       <c r="I124">
-        <v>0.376500439033506</v>
+        <v>0.53708325709935101</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -4095,7 +4095,7 @@
         <v>4.0432283757956898E-2</v>
       </c>
       <c r="I125">
-        <v>0.34242728096347302</v>
+        <v>0.54319964312374203</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -4124,7 +4124,7 @@
         <v>4.0420556095911803E-2</v>
       </c>
       <c r="I126">
-        <v>0.313152096286262</v>
+        <v>0.55320754078960699</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -4153,7 +4153,7 @@
         <v>4.0475403858868497E-2</v>
       </c>
       <c r="I127">
-        <v>0.29094842505644802</v>
+        <v>0.53183270853266595</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -4182,7 +4182,7 @@
         <v>4.0691206324752399E-2</v>
       </c>
       <c r="I128">
-        <v>0.297555852289761</v>
+        <v>0.53492335140172798</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -4211,7 +4211,7 @@
         <v>4.0479476085913499E-2</v>
       </c>
       <c r="I129">
-        <v>0.30852858318648502</v>
+        <v>0.55858247652175996</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -4240,7 +4240,7 @@
         <v>4.0466433681525603E-2</v>
       </c>
       <c r="I130">
-        <v>0.28533602986519102</v>
+        <v>0.54823975865849695</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -4269,7 +4269,7 @@
         <v>4.0337007356705402E-2</v>
       </c>
       <c r="I131">
-        <v>0.28863299187485703</v>
+        <v>0.54465286625354603</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
@@ -4298,7 +4298,7 @@
         <v>4.0488730088522197E-2</v>
       </c>
       <c r="I132">
-        <v>0.31450438307718298</v>
+        <v>0.58935684110750697</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -4327,7 +4327,7 @@
         <v>4.0568718769069603E-2</v>
       </c>
       <c r="I133">
-        <v>0.30305683297392699</v>
+        <v>0.56556761908724196</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -4356,7 +4356,7 @@
         <v>4.0656314020364903E-2</v>
       </c>
       <c r="I134">
-        <v>0.29913674471820301</v>
+        <v>0.54431071606721204</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -4385,7 +4385,7 @@
         <v>4.0498313176113E-2</v>
       </c>
       <c r="I135">
-        <v>0.34983148616021897</v>
+        <v>0.52404383103479701</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -4414,7 +4414,7 @@
         <v>4.0509917781658897E-2</v>
       </c>
       <c r="I136">
-        <v>0.32235673176001201</v>
+        <v>0.51226393923762903</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -4443,7 +4443,7 @@
         <v>4.0518015669222397E-2</v>
       </c>
       <c r="I137">
-        <v>0.29876415562560099</v>
+        <v>0.51196794401977597</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -4472,7 +4472,7 @@
         <v>4.0509596715445302E-2</v>
       </c>
       <c r="I138">
-        <v>0.27711193684562702</v>
+        <v>0.496482084544136</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -4501,7 +4501,7 @@
         <v>4.0487473643912399E-2</v>
       </c>
       <c r="I139">
-        <v>0.26490434344325298</v>
+        <v>0.50854920242172597</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -4530,7 +4530,7 @@
         <v>4.0517119847981002E-2</v>
       </c>
       <c r="I140">
-        <v>0.26460117570383601</v>
+        <v>0.49822181927655901</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
@@ -4559,7 +4559,7 @@
         <v>4.0501943562167297E-2</v>
       </c>
       <c r="I141">
-        <v>0.24898446027329099</v>
+        <v>0.48414234267293399</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -4588,7 +4588,7 @@
         <v>4.0567723047911203E-2</v>
       </c>
       <c r="I142">
-        <v>0.261112291283774</v>
+        <v>0.509170553169355</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
@@ -4617,7 +4617,7 @@
         <v>4.0516747870774202E-2</v>
       </c>
       <c r="I143">
-        <v>0.25071498120324398</v>
+        <v>0.52513247407998698</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -4646,7 +4646,7 @@
         <v>4.05109594930263E-2</v>
       </c>
       <c r="I144">
-        <v>0.23688380796883601</v>
+        <v>0.52711713127086701</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -4675,7 +4675,7 @@
         <v>4.0426910989507403E-2</v>
       </c>
       <c r="I145">
-        <v>0.26174465221478699</v>
+        <v>0.66981328111496197</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -4704,7 +4704,7 @@
         <v>4.0468134657409699E-2</v>
       </c>
       <c r="I146">
-        <v>0.27825411533336802</v>
+        <v>0.63043146728787003</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -4733,7 +4733,7 @@
         <v>4.04100526973536E-2</v>
       </c>
       <c r="I147">
-        <v>0.28034247007922802</v>
+        <v>0.59976315975592998</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
@@ -4762,7 +4762,7 @@
         <v>4.05142950431003E-2</v>
       </c>
       <c r="I148">
-        <v>0.45113983155799098</v>
+        <v>0.57121573872728104</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -4791,7 +4791,7 @@
         <v>4.0517780985909302E-2</v>
       </c>
       <c r="I149">
-        <v>0.39993383494673701</v>
+        <v>0.55499433298782597</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -4820,7 +4820,7 @@
         <v>4.0530414429008003E-2</v>
       </c>
       <c r="I150">
-        <v>0.36220584780041698</v>
+        <v>0.53305486925052403</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -4849,7 +4849,7 @@
         <v>4.0530439021751102E-2</v>
       </c>
       <c r="I151">
-        <v>0.32877742016975298</v>
+        <v>0.52196753664427797</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
@@ -4878,7 +4878,7 @@
         <v>4.0499578227503601E-2</v>
       </c>
       <c r="I152">
-        <v>0.310508709648602</v>
+        <v>0.51534686939917895</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -4907,7 +4907,7 @@
         <v>4.0499602133718102E-2</v>
       </c>
       <c r="I153">
-        <v>0.286637493631693</v>
+        <v>0.50206801508401999</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -4936,7 +4936,7 @@
         <v>4.05168834881523E-2</v>
       </c>
       <c r="I154">
-        <v>0.27494010931049601</v>
+        <v>0.52711728135184999</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -4965,7 +4965,7 @@
         <v>4.0490189271041498E-2</v>
       </c>
       <c r="I155">
-        <v>0.26807239579953501</v>
+        <v>0.532260150417323</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -4994,7 +4994,7 @@
         <v>4.0473364121900397E-2</v>
       </c>
       <c r="I156">
-        <v>0.25456229177040801</v>
+        <v>0.54737751655518196</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -5023,7 +5023,7 @@
         <v>4.0435863273217097E-2</v>
       </c>
       <c r="I157">
-        <v>0.28034262829976597</v>
+        <v>0.54112794868402303</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -5052,7 +5052,7 @@
         <v>4.0456003309074499E-2</v>
       </c>
       <c r="I158">
-        <v>0.28579086772227202</v>
+        <v>0.52239073802087799</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -5081,7 +5081,7 @@
         <v>4.0440218285864402E-2</v>
       </c>
       <c r="I159">
-        <v>0.30211214563011901</v>
+        <v>0.56560062687204604</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -5110,7 +5110,7 @@
         <v>4.0460255316372401E-2</v>
       </c>
       <c r="I160">
-        <v>0.29530945684697801</v>
+        <v>0.61430055781222703</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
@@ -5139,7 +5139,7 @@
         <v>4.0461615652767499E-2</v>
       </c>
       <c r="I161">
-        <v>0.27538208316999802</v>
+        <v>0.63665973497815298</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -5168,7 +5168,7 @@
         <v>4.0485108726504397E-2</v>
       </c>
       <c r="I162">
-        <v>0.32239406911805102</v>
+        <v>0.634319617836688</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -5197,7 +5197,7 @@
         <v>4.0499952309068797E-2</v>
       </c>
       <c r="I163">
-        <v>0.37985517532841301</v>
+        <v>0.63064883772235303</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
@@ -5226,7 +5226,7 @@
         <v>4.05483799940018E-2</v>
       </c>
       <c r="I164">
-        <v>0.407825618142451</v>
+        <v>0.70132246569182699</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
@@ -5255,7 +5255,7 @@
         <v>4.04543062969435E-2</v>
       </c>
       <c r="I165">
-        <v>0.40485137757248102</v>
+        <v>0.66504432253019696</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
@@ -5284,7 +5284,7 @@
         <v>4.05701878018506E-2</v>
       </c>
       <c r="I166">
-        <v>0.40020795652055402</v>
+        <v>0.65286820418497105</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -5313,7 +5313,7 @@
         <v>4.0343975368168E-2</v>
       </c>
       <c r="I167">
-        <v>0.49434320088406403</v>
+        <v>0.62485600775876504</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
@@ -5342,7 +5342,7 @@
         <v>4.0304000059875097E-2</v>
       </c>
       <c r="I168">
-        <v>0.444773950929648</v>
+        <v>0.59336787848703199</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -5371,7 +5371,7 @@
         <v>4.0372420894020503E-2</v>
       </c>
       <c r="I169">
-        <v>0.42872689203570902</v>
+        <v>0.57948499459012504</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -5400,7 +5400,7 @@
         <v>4.0423201018770602E-2</v>
       </c>
       <c r="I170">
-        <v>0.392935030432221</v>
+        <v>0.55774852822225296</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
@@ -5429,7 +5429,7 @@
         <v>4.0405287899560299E-2</v>
       </c>
       <c r="I171">
-        <v>0.35457543922020102</v>
+        <v>0.56834325121360296</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -5458,7 +5458,7 @@
         <v>4.0322561456389197E-2</v>
       </c>
       <c r="I172">
-        <v>0.33829285895511702</v>
+        <v>0.55259189705915901</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -5487,7 +5487,7 @@
         <v>4.02929938162341E-2</v>
       </c>
       <c r="I173">
-        <v>0.313573420734089</v>
+        <v>0.60151051655724597</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -5516,7 +5516,7 @@
         <v>4.02680309740212E-2</v>
       </c>
       <c r="I174">
-        <v>0.32550405120004899</v>
+        <v>0.59828324930972399</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -5545,7 +5545,7 @@
         <v>4.0271857551171998E-2</v>
       </c>
       <c r="I175">
-        <v>0.30784780469543999</v>
+        <v>0.63110671445418998</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
@@ -5574,7 +5574,7 @@
         <v>4.0223663790814899E-2</v>
       </c>
       <c r="I176">
-        <v>0.364304901528965</v>
+        <v>0.63518386648141201</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
@@ -5603,7 +5603,7 @@
         <v>4.0243613948369797E-2</v>
       </c>
       <c r="I177">
-        <v>0.36043284640460099</v>
+        <v>0.63333673666319701</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
@@ -5632,7 +5632,7 @@
         <v>4.0314553642649999E-2</v>
       </c>
       <c r="I178">
-        <v>0.40078568502916301</v>
+        <v>0.66538680066276101</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
@@ -5661,7 +5661,7 @@
         <v>4.0204336972128503E-2</v>
       </c>
       <c r="I179">
-        <v>0.40594854423827598</v>
+        <v>0.63027308861766695</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
@@ -5690,7 +5690,7 @@
         <v>4.0113485829036601E-2</v>
       </c>
       <c r="I180">
-        <v>0.40360542200718702</v>
+        <v>0.685266125609445</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
@@ -5719,7 +5719,7 @@
         <v>4.0243880898409599E-2</v>
       </c>
       <c r="I181">
-        <v>0.44522959449622501</v>
+        <v>0.69579192562175196</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
@@ -5748,7 +5748,7 @@
         <v>4.0221306585537103E-2</v>
       </c>
       <c r="I182">
-        <v>0.399734166235653</v>
+        <v>0.69824370236942901</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
@@ -5777,7 +5777,7 @@
         <v>4.0409013462085801E-2</v>
       </c>
       <c r="I183">
-        <v>0.47207966290777997</v>
+        <v>0.69634297716659099</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
@@ -5806,7 +5806,7 @@
         <v>4.0257050124659501E-2</v>
       </c>
       <c r="I184">
-        <v>0.48661640376042598</v>
+        <v>0.74719561194202899</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
@@ -5835,7 +5835,7 @@
         <v>4.0162547513185202E-2</v>
       </c>
       <c r="I185">
-        <v>0.49003426789856702</v>
+        <v>0.69526930190770497</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
@@ -5864,7 +5864,7 @@
         <v>4.0244926581978098E-2</v>
       </c>
       <c r="I186">
-        <v>0.48738354184923199</v>
+        <v>0.70892108921780395</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
@@ -5893,7 +5893,7 @@
         <v>4.0130823867760401E-2</v>
       </c>
       <c r="I187">
-        <v>0.56079128250542298</v>
+        <v>0.68169906230895805</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
@@ -5922,7 +5922,7 @@
         <v>4.0141042513094E-2</v>
       </c>
       <c r="I188">
-        <v>0.48588940217522802</v>
+        <v>0.66117224469976399</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
@@ -5951,7 +5951,7 @@
         <v>4.0183022034079398E-2</v>
       </c>
       <c r="I189">
-        <v>0.505059110737758</v>
+        <v>0.62455732838224698</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
@@ -5980,7 +5980,7 @@
         <v>4.0136813092777897E-2</v>
       </c>
       <c r="I190">
-        <v>0.46720361155291301</v>
+        <v>1.6675472371637801</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
@@ -6009,7 +6009,7 @@
         <v>4.0120942049019802E-2</v>
       </c>
       <c r="I191">
-        <v>0.43963873716132501</v>
+        <v>1.4329310664768</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
@@ -6038,7 +6038,7 @@
         <v>4.0127754145021802E-2</v>
       </c>
       <c r="I192">
-        <v>0.39256185643597002</v>
+        <v>1.3138643628836699</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
@@ -6067,7 +6067,7 @@
         <v>4.0110809079312901E-2</v>
       </c>
       <c r="I193">
-        <v>2.7832037881725702</v>
+        <v>1.15774216007083</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
@@ -6096,7 +6096,7 @@
         <v>4.0146840946407497E-2</v>
       </c>
       <c r="I194">
-        <v>2.0557814412743398</v>
+        <v>1.1781036455326901</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
@@ -6125,7 +6125,7 @@
         <v>4.0038525251966502E-2</v>
       </c>
       <c r="I195">
-        <v>1.7287295640557001</v>
+        <v>1.0543736014573299</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
@@ -6154,7 +6154,7 @@
         <v>4.0005818409089199E-2</v>
       </c>
       <c r="I196">
-        <v>1.3428569092054701</v>
+        <v>0.95338589941475005</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
@@ -6183,7 +6183,7 @@
         <v>3.9742157458295402E-2</v>
       </c>
       <c r="I197">
-        <v>1.3904181996174101</v>
+        <v>0.89082654806934702</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
@@ -6212,7 +6212,7 @@
         <v>3.98051518839743E-2</v>
       </c>
       <c r="I198">
-        <v>1.11419369145011</v>
+        <v>0.82230486211444198</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
@@ -6241,7 +6241,7 @@
         <v>3.98668209956662E-2</v>
       </c>
       <c r="I199">
-        <v>0.91143467320287197</v>
+        <v>0.78954772828131203</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
@@ -6270,7 +6270,7 @@
         <v>3.9976004182503203E-2</v>
       </c>
       <c r="I200">
-        <v>0.79606193874514897</v>
+        <v>0.80485377041204398</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
@@ -6299,7 +6299,7 @@
         <v>3.9920039314419203E-2</v>
       </c>
       <c r="I201">
-        <v>0.67867528625705198</v>
+        <v>0.74350057088333199</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
@@ -6328,7 +6328,7 @@
         <v>3.9849419812588598E-2</v>
       </c>
       <c r="I202">
-        <v>0.62587561523418</v>
+        <v>0.70218188935953996</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
@@ -6357,7 +6357,7 @@
         <v>3.9729621673674602E-2</v>
       </c>
       <c r="I203">
-        <v>0.65027959174648398</v>
+        <v>0.74148866056881202</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
@@ -6386,7 +6386,7 @@
         <v>3.9731908293277302E-2</v>
       </c>
       <c r="I204">
-        <v>0.55528309890383998</v>
+        <v>0.72405627081496704</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
@@ -6415,7 +6415,7 @@
         <v>3.9768474087676503E-2</v>
       </c>
       <c r="I205">
-        <v>0.49554940574453399</v>
+        <v>0.70994844616855302</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
@@ -6444,7 +6444,7 @@
         <v>3.9662718197324101E-2</v>
       </c>
       <c r="I206">
-        <v>0.55229543375213097</v>
+        <v>0.67539373728457497</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
@@ -6473,7 +6473,7 @@
         <v>3.9671645681036899E-2</v>
       </c>
       <c r="I207">
-        <v>0.52674748330647703</v>
+        <v>0.63922487576112796</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
@@ -6502,7 +6502,7 @@
         <v>3.9666568419565798E-2</v>
       </c>
       <c r="I208">
-        <v>0.50651679621714196</v>
+        <v>0.62327478736337505</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
@@ -6531,7 +6531,7 @@
         <v>3.96635671425545E-2</v>
       </c>
       <c r="I209">
-        <v>0.45864670036322502</v>
+        <v>0.60156488612779402</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
@@ -6560,7 +6560,7 @@
         <v>3.9668062150389899E-2</v>
       </c>
       <c r="I210">
-        <v>0.41109844179183003</v>
+        <v>0.57694185711113699</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
@@ -6589,7 +6589,7 @@
         <v>3.9661711622805997E-2</v>
       </c>
       <c r="I211">
-        <v>0.39096146056286002</v>
+        <v>0.56824536655994895</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
@@ -6618,7 +6618,7 @@
         <v>3.9643109280154201E-2</v>
       </c>
       <c r="I212">
-        <v>0.36437031222194599</v>
+        <v>0.56209187500624502</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
@@ -6647,7 +6647,7 @@
         <v>3.9635010864136899E-2</v>
       </c>
       <c r="I213">
-        <v>0.33535190648684698</v>
+        <v>0.54318442917038201</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
@@ -6676,7 +6676,7 @@
         <v>3.9564171873053798E-2</v>
       </c>
       <c r="I214">
-        <v>0.325392796616851</v>
+        <v>0.55199228176889603</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
@@ -6705,7 +6705,7 @@
         <v>3.9575328683980698E-2</v>
       </c>
       <c r="I215">
-        <v>0.318437275948036</v>
+        <v>0.57759101814209302</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
@@ -6734,7 +6734,7 @@
         <v>3.9544343194512402E-2</v>
       </c>
       <c r="I216">
-        <v>0.29753932409315398</v>
+        <v>0.62605353706744304</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
@@ -6763,7 +6763,7 @@
         <v>3.9426282904250903E-2</v>
       </c>
       <c r="I217">
-        <v>0.30718547913243199</v>
+        <v>0.602684539157749</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
@@ -6792,7 +6792,7 @@
         <v>3.9301907953157897E-2</v>
       </c>
       <c r="I218">
-        <v>0.33610138423842001</v>
+        <v>0.58394356364267097</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
@@ -6821,7 +6821,7 @@
         <v>3.94580235208234E-2</v>
       </c>
       <c r="I219">
-        <v>0.39443303127465601</v>
+        <v>0.59051858838443705</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
@@ -6850,7 +6850,7 @@
         <v>3.9379083648224698E-2</v>
       </c>
       <c r="I220">
-        <v>0.36571865373978801</v>
+        <v>0.60221349100545296</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
@@ -6879,7 +6879,7 @@
         <v>3.92866172482935E-2</v>
       </c>
       <c r="I221">
-        <v>0.34348008551970199</v>
+        <v>0.57750702736136295</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
@@ -6908,7 +6908,7 @@
         <v>3.9424781934948798E-2</v>
       </c>
       <c r="I222">
-        <v>0.35120220322754803</v>
+        <v>0.56781385563173103</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
@@ -6937,7 +6937,7 @@
         <v>3.9611330563128197E-2</v>
       </c>
       <c r="I223">
-        <v>0.36515108874897401</v>
+        <v>0.54939380318789499</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
@@ -6966,7 +6966,7 @@
         <v>3.9552694429925497E-2</v>
       </c>
       <c r="I224">
-        <v>0.33600436665175798</v>
+        <v>0.56380916058328401</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
@@ -6995,7 +6995,7 @@
         <v>3.94326899818042E-2</v>
       </c>
       <c r="I225">
-        <v>0.32490257464737199</v>
+        <v>0.55199428931484695</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
@@ -7024,7 +7024,7 @@
         <v>3.95037932332679E-2</v>
       </c>
       <c r="I226">
-        <v>0.30432355098126002</v>
+        <v>0.55170090387223203</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
@@ -7053,7 +7053,7 @@
         <v>3.9311237085224902E-2</v>
       </c>
       <c r="I227">
-        <v>0.320370769557628</v>
+        <v>0.61866481124980999</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
@@ -7082,7 +7082,7 @@
         <v>3.92260964719452E-2</v>
       </c>
       <c r="I228">
-        <v>0.307187695436203</v>
+        <v>0.587493506002013</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
@@ -7111,7 +7111,7 @@
         <v>3.9324158649941397E-2</v>
       </c>
       <c r="I229">
-        <v>0.306863887333437</v>
+        <v>0.64681754828589</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
@@ -7140,7 +7140,7 @@
         <v>3.9594849023863801E-2</v>
       </c>
       <c r="I230">
-        <v>0.38523614867876299</v>
+        <v>0.61448932555704106</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
@@ -7169,7 +7169,7 @@
         <v>3.9582964027063801E-2</v>
       </c>
       <c r="I231">
-        <v>0.34763861959453701</v>
+        <v>0.59940702461308504</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
@@ -7198,7 +7198,7 @@
         <v>3.9256670134426297E-2</v>
       </c>
       <c r="I232">
-        <v>0.42086294077056902</v>
+        <v>0.57092979303178604</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
@@ -7227,7 +7227,7 @@
         <v>3.9324213008088103E-2</v>
       </c>
       <c r="I233">
-        <v>0.38008713122354798</v>
+        <v>0.55199289604391699</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
@@ -7256,7 +7256,7 @@
         <v>3.9213542877347102E-2</v>
       </c>
       <c r="I234">
-        <v>0.36177878115551199</v>
+        <v>0.536334309890099</v>
       </c>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
@@ -7285,7 +7285,7 @@
         <v>3.9209964599998502E-2</v>
       </c>
       <c r="I235">
-        <v>0.32845082857131802</v>
+        <v>0.51851695869810999</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
@@ -7314,7 +7314,7 @@
         <v>3.9156461241587101E-2</v>
       </c>
       <c r="I236">
-        <v>0.30718615728295001</v>
+        <v>2.3831902739222901</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
@@ -7343,7 +7343,7 @@
         <v>3.9086537387403301E-2</v>
       </c>
       <c r="I237">
-        <v>0.29014449196528902</v>
+        <v>2.24006196694156</v>
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
@@ -7372,7 +7372,7 @@
         <v>3.9157141122953397E-2</v>
       </c>
       <c r="I238">
-        <v>0.27134983645753802</v>
+        <v>1.85769801923377</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
@@ -7401,7 +7401,7 @@
         <v>3.8360562714448702E-2</v>
       </c>
       <c r="I239">
-        <v>5.6820858817177804</v>
+        <v>1.6719388613819799</v>
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
@@ -7430,7 +7430,7 @@
         <v>3.80248151289687E-2</v>
       </c>
       <c r="I240">
-        <v>5.0203676157380803</v>
+        <v>1.834890879402</v>
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
@@ -7459,7 +7459,7 @@
         <v>3.8045576314815102E-2</v>
       </c>
       <c r="I241">
-        <v>3.45353193066506</v>
+        <v>1.5527814661572801</v>
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
@@ -7488,7 +7488,7 @@
         <v>3.8036969356628897E-2</v>
       </c>
       <c r="I242">
-        <v>2.7978695561992599</v>
+        <v>1.3618563776586801</v>
       </c>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.25">
@@ -7517,7 +7517,7 @@
         <v>3.80365209615404E-2</v>
       </c>
       <c r="I243">
-        <v>3.36931453931264</v>
+        <v>1.2211522428046699</v>
       </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
@@ -7546,7 +7546,7 @@
         <v>3.8055607110235597E-2</v>
       </c>
       <c r="I244">
-        <v>2.4136202816415402</v>
+        <v>1.13849320034686</v>
       </c>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
@@ -7575,7 +7575,7 @@
         <v>3.81000467017042E-2</v>
       </c>
       <c r="I245">
-        <v>1.8571427933696201</v>
+        <v>1.0132148055047401</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
@@ -7604,7 +7604,7 @@
         <v>3.8197592262906803E-2</v>
       </c>
       <c r="I246">
-        <v>1.4937028001068899</v>
+        <v>0.93646459554444905</v>
       </c>
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.25">
@@ -7633,7 +7633,7 @@
         <v>3.8064062853987397E-2</v>
       </c>
       <c r="I247">
-        <v>1.2986567672360301</v>
+        <v>0.85775975632384904</v>
       </c>
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.25">
@@ -7662,7 +7662,7 @@
         <v>3.8076485290018398E-2</v>
       </c>
       <c r="I248">
-        <v>1.0290942420940099</v>
+        <v>0.863300152691719</v>
       </c>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
@@ -7691,7 +7691,7 @@
         <v>3.79921982522003E-2</v>
       </c>
       <c r="I249">
-        <v>0.87945593870822802</v>
+        <v>1.1115487963892201</v>
       </c>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
@@ -7720,7 +7720,7 @@
         <v>3.79416335219648E-2</v>
       </c>
       <c r="I250">
-        <v>0.73824179956874902</v>
+        <v>1.06680910582024</v>
       </c>
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.25">
@@ -7749,7 +7749,7 @@
         <v>3.7740510054703101E-2</v>
       </c>
       <c r="I251">
-        <v>0.74777715363754504</v>
+        <v>1.0186691867192099</v>
       </c>
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.25">
@@ -7778,7 +7778,7 @@
         <v>3.7451684484177197E-2</v>
       </c>
       <c r="I252">
-        <v>1.23803072675433</v>
+        <v>0.94148888190817503</v>
       </c>
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.25">
@@ -7807,7 +7807,7 @@
         <v>3.7364680324472703E-2</v>
       </c>
       <c r="I253">
-        <v>1.1405716682609801</v>
+        <v>0.88018867939003498</v>
       </c>
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.25">
@@ -7836,7 +7836,7 @@
         <v>3.7460166900804101E-2</v>
       </c>
       <c r="I254">
-        <v>1.0401769119711699</v>
+        <v>0.80688055627925404</v>
       </c>
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.25">
@@ -7865,7 +7865,7 @@
         <v>3.7403774483407398E-2</v>
       </c>
       <c r="I255">
-        <v>0.88889131475670602</v>
+        <v>0.77559553711299001</v>
       </c>
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>